<commit_message>
[main] Update resources and fix typo.
</commit_message>
<xml_diff>
--- a/Resources/Part1/Part1_Resources.xlsx
+++ b/Resources/Part1/Part1_Resources.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_dev\Repository\CSC_MS\Part1\Rsc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_dev\Repository\CSC_MS\Resources\Part1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CC0047-6CBB-4B0F-8CC7-A53BE256974B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556376CD-4A54-4455-BDD5-D39DA9AFA9EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13545" xr2:uid="{5FC90DE4-2FBD-4B96-ADE9-01AE3F36C35E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
   <si>
     <t>SyRS</t>
     <phoneticPr fontId="1"/>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>The gantt chart for each of deliverables by division.</t>
+  </si>
+  <si>
+    <t>D.AT</t>
   </si>
 </sst>
 </file>
@@ -1183,7 +1186,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1192,44 +1231,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1548,7 +1551,7 @@
   <dimension ref="B2:AA30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1569,46 +1572,46 @@
     </row>
     <row r="4" spans="2:27" ht="32.25" customHeight="1">
       <c r="D4" s="6"/>
-      <c r="E4" s="105" t="s">
+      <c r="E4" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="106"/>
-      <c r="G4" s="105" t="s">
+      <c r="F4" s="105"/>
+      <c r="G4" s="104" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="106"/>
-      <c r="I4" s="105" t="s">
+      <c r="H4" s="105"/>
+      <c r="I4" s="104" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="106"/>
-      <c r="K4" s="105" t="s">
+      <c r="J4" s="105"/>
+      <c r="K4" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="L4" s="106"/>
-      <c r="N4" s="105" t="s">
+      <c r="L4" s="105"/>
+      <c r="N4" s="104" t="s">
         <v>28</v>
       </c>
-      <c r="O4" s="106"/>
-      <c r="P4" s="103" t="s">
+      <c r="O4" s="105"/>
+      <c r="P4" s="115" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="104"/>
-      <c r="R4" s="103" t="s">
+      <c r="Q4" s="116"/>
+      <c r="R4" s="115" t="s">
         <v>17</v>
       </c>
-      <c r="S4" s="104"/>
-      <c r="T4" s="103" t="s">
+      <c r="S4" s="116"/>
+      <c r="T4" s="115" t="s">
         <v>18</v>
       </c>
-      <c r="U4" s="104"/>
-      <c r="V4" s="103" t="s">
+      <c r="U4" s="116"/>
+      <c r="V4" s="115" t="s">
         <v>26</v>
       </c>
-      <c r="W4" s="104"/>
-      <c r="Y4" s="103" t="s">
+      <c r="W4" s="116"/>
+      <c r="Y4" s="115" t="s">
         <v>31</v>
       </c>
-      <c r="Z4" s="104"/>
+      <c r="Z4" s="116"/>
     </row>
     <row r="5" spans="2:27">
       <c r="D5" s="1"/>
@@ -1650,10 +1653,10 @@
       <c r="Z6" s="4"/>
     </row>
     <row r="7" spans="2:27" ht="15.75" thickBot="1">
-      <c r="B7" s="107" t="s">
+      <c r="B7" s="111" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="115" t="s">
+      <c r="C7" s="108" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="69"/>
@@ -1682,8 +1685,8 @@
       <c r="AA7" s="3"/>
     </row>
     <row r="8" spans="2:27">
-      <c r="B8" s="108"/>
-      <c r="C8" s="115"/>
+      <c r="B8" s="112"/>
+      <c r="C8" s="108"/>
       <c r="D8" s="73"/>
       <c r="E8" s="74"/>
       <c r="F8" s="75"/>
@@ -1710,10 +1713,10 @@
       <c r="AA8" s="3"/>
     </row>
     <row r="9" spans="2:27" ht="15.75" thickBot="1">
-      <c r="B9" s="109" t="s">
+      <c r="B9" s="113" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="116" t="s">
+      <c r="C9" s="109" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="14"/>
@@ -1742,8 +1745,8 @@
       <c r="AA9" s="3"/>
     </row>
     <row r="10" spans="2:27">
-      <c r="B10" s="110"/>
-      <c r="C10" s="116"/>
+      <c r="B10" s="114"/>
+      <c r="C10" s="109"/>
       <c r="D10" s="14"/>
       <c r="E10" s="19" t="s">
         <v>5</v>
@@ -1778,8 +1781,8 @@
       <c r="AA10" s="3"/>
     </row>
     <row r="11" spans="2:27" ht="15.75" thickBot="1">
-      <c r="B11" s="110"/>
-      <c r="C11" s="116" t="s">
+      <c r="B11" s="114"/>
+      <c r="C11" s="109" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="14"/>
@@ -1808,8 +1811,8 @@
       <c r="AA11" s="3"/>
     </row>
     <row r="12" spans="2:27">
-      <c r="B12" s="110"/>
-      <c r="C12" s="116"/>
+      <c r="B12" s="114"/>
+      <c r="C12" s="109"/>
       <c r="D12" s="14"/>
       <c r="E12" s="17"/>
       <c r="F12" s="16"/>
@@ -1844,8 +1847,8 @@
       <c r="AA12" s="3"/>
     </row>
     <row r="13" spans="2:27" ht="15.75" thickBot="1">
-      <c r="B13" s="110"/>
-      <c r="C13" s="117" t="s">
+      <c r="B13" s="114"/>
+      <c r="C13" s="110" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="14"/>
@@ -1874,8 +1877,8 @@
       <c r="AA13" s="3"/>
     </row>
     <row r="14" spans="2:27" ht="30">
-      <c r="B14" s="110"/>
-      <c r="C14" s="116"/>
+      <c r="B14" s="114"/>
+      <c r="C14" s="109"/>
       <c r="D14" s="14"/>
       <c r="E14" s="17"/>
       <c r="F14" s="16"/>
@@ -1918,10 +1921,10 @@
       <c r="AA14" s="3"/>
     </row>
     <row r="15" spans="2:27" ht="15.75" thickBot="1">
-      <c r="B15" s="111" t="s">
+      <c r="B15" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="113" t="s">
+      <c r="C15" s="106" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="82"/>
@@ -1950,8 +1953,8 @@
       <c r="AA15" s="3"/>
     </row>
     <row r="16" spans="2:27" ht="16.5">
-      <c r="B16" s="112"/>
-      <c r="C16" s="114"/>
+      <c r="B16" s="103"/>
+      <c r="C16" s="107"/>
       <c r="D16" s="86"/>
       <c r="E16" s="29"/>
       <c r="F16" s="30"/>
@@ -1990,8 +1993,8 @@
       <c r="AA16" s="3"/>
     </row>
     <row r="17" spans="2:27" ht="15.75" thickBot="1">
-      <c r="B17" s="112"/>
-      <c r="C17" s="113" t="s">
+      <c r="B17" s="103"/>
+      <c r="C17" s="106" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="86"/>
@@ -2020,8 +2023,8 @@
       <c r="AA17" s="3"/>
     </row>
     <row r="18" spans="2:27" ht="16.5">
-      <c r="B18" s="112"/>
-      <c r="C18" s="114"/>
+      <c r="B18" s="103"/>
+      <c r="C18" s="107"/>
       <c r="D18" s="86"/>
       <c r="E18" s="29"/>
       <c r="F18" s="30"/>
@@ -2060,8 +2063,8 @@
       <c r="AA18" s="3"/>
     </row>
     <row r="19" spans="2:27" ht="15.75" thickBot="1">
-      <c r="B19" s="112"/>
-      <c r="C19" s="113" t="s">
+      <c r="B19" s="103"/>
+      <c r="C19" s="106" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="86"/>
@@ -2090,14 +2093,14 @@
       <c r="AA19" s="3"/>
     </row>
     <row r="20" spans="2:27" ht="16.5">
-      <c r="B20" s="112"/>
-      <c r="C20" s="114"/>
+      <c r="B20" s="103"/>
+      <c r="C20" s="107"/>
       <c r="D20" s="87"/>
       <c r="E20" s="88" t="s">
         <v>5</v>
       </c>
       <c r="F20" s="89" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="G20" s="90"/>
       <c r="H20" s="91"/>
@@ -2200,10 +2203,10 @@
         <v>32</v>
       </c>
       <c r="D25" s="13"/>
-      <c r="E25" s="102" t="s">
+      <c r="E25" s="117" t="s">
         <v>37</v>
       </c>
-      <c r="I25" s="102"/>
+      <c r="I25" s="117"/>
       <c r="AA25" s="3"/>
     </row>
     <row r="26" spans="2:27">
@@ -2211,44 +2214,60 @@
         <v>33</v>
       </c>
       <c r="D26" s="10"/>
-      <c r="E26" s="102"/>
-      <c r="I26" s="102"/>
+      <c r="E26" s="117"/>
+      <c r="I26" s="117"/>
     </row>
     <row r="27" spans="2:27" ht="15.75" thickBot="1">
       <c r="B27" t="s">
         <v>34</v>
       </c>
       <c r="D27" s="98"/>
-      <c r="E27" s="102" t="s">
+      <c r="E27" s="117" t="s">
         <v>38</v>
       </c>
-      <c r="I27" s="102"/>
+      <c r="I27" s="117"/>
     </row>
     <row r="28" spans="2:27">
       <c r="B28" t="s">
         <v>35</v>
       </c>
       <c r="D28" s="99"/>
-      <c r="E28" s="102"/>
-      <c r="I28" s="102"/>
+      <c r="E28" s="117"/>
+      <c r="I28" s="117"/>
     </row>
     <row r="29" spans="2:27" ht="15.75" thickBot="1">
       <c r="B29" t="s">
         <v>36</v>
       </c>
       <c r="D29" s="100"/>
-      <c r="E29" s="102" t="s">
+      <c r="E29" s="117" t="s">
         <v>39</v>
       </c>
-      <c r="I29" s="102"/>
+      <c r="I29" s="117"/>
     </row>
     <row r="30" spans="2:27">
       <c r="D30" s="101"/>
-      <c r="E30" s="102"/>
-      <c r="I30" s="102"/>
+      <c r="E30" s="117"/>
+      <c r="I30" s="117"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B14"/>
     <mergeCell ref="B15:B20"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G4:H4"/>
@@ -2259,22 +2278,6 @@
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="C17:C18"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B14"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="I25:I26"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="I29:I30"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="E29:E30"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>